<commit_message>
reativei o comando de modelo no final do script
</commit_message>
<xml_diff>
--- a/output/classeGenotiposCS_2022-06-17.xlsx
+++ b/output/classeGenotiposCS_2022-06-17.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1946"/>
+  <dimension ref="A1:E1990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -45119,6 +45119,1018 @@
         </is>
       </c>
     </row>
+    <row r="1947">
+      <c r="A1947" t="inlineStr">
+        <is>
+          <t>AG8700PRO3</t>
+        </is>
+      </c>
+      <c r="B1947" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1947">
+        <v>5.73</v>
+      </c>
+      <c r="D1947">
+        <v>6</v>
+      </c>
+      <c r="E1947" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1948">
+      <c r="A1948" t="inlineStr">
+        <is>
+          <t>AS1633PRO3</t>
+        </is>
+      </c>
+      <c r="B1948" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1948">
+        <v>4.86</v>
+      </c>
+      <c r="D1948">
+        <v>6</v>
+      </c>
+      <c r="E1948" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1949">
+      <c r="A1949" t="inlineStr">
+        <is>
+          <t>AS1820PRO3</t>
+        </is>
+      </c>
+      <c r="B1949" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1949">
+        <v>3.99</v>
+      </c>
+      <c r="D1949">
+        <v>6</v>
+      </c>
+      <c r="E1949" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1950">
+      <c r="A1950" t="inlineStr">
+        <is>
+          <t>AS1868PRO3</t>
+        </is>
+      </c>
+      <c r="B1950" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1950">
+        <v>4.34</v>
+      </c>
+      <c r="D1950">
+        <v>6</v>
+      </c>
+      <c r="E1950" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1951">
+      <c r="A1951" t="inlineStr">
+        <is>
+          <t>B2401PWU</t>
+        </is>
+      </c>
+      <c r="B1951" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1951">
+        <v>4.51</v>
+      </c>
+      <c r="D1951">
+        <v>6</v>
+      </c>
+      <c r="E1951" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1952">
+      <c r="A1952" t="inlineStr">
+        <is>
+          <t>B2620PWU</t>
+        </is>
+      </c>
+      <c r="B1952" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1952">
+        <v>5.21</v>
+      </c>
+      <c r="D1952">
+        <v>6</v>
+      </c>
+      <c r="E1952" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1953">
+      <c r="A1953" t="inlineStr">
+        <is>
+          <t>DKB255PRO3</t>
+        </is>
+      </c>
+      <c r="B1953" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1953">
+        <v>3.99</v>
+      </c>
+      <c r="D1953">
+        <v>6</v>
+      </c>
+      <c r="E1953" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1954">
+      <c r="A1954" t="inlineStr">
+        <is>
+          <t>DKB335PRO3</t>
+        </is>
+      </c>
+      <c r="B1954" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1954">
+        <v>4.16</v>
+      </c>
+      <c r="D1954">
+        <v>6</v>
+      </c>
+      <c r="E1954" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1955">
+      <c r="A1955" t="inlineStr">
+        <is>
+          <t>DKB360PRO3</t>
+        </is>
+      </c>
+      <c r="B1955" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1955">
+        <v>4.51</v>
+      </c>
+      <c r="D1955">
+        <v>6</v>
+      </c>
+      <c r="E1955" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1956">
+      <c r="A1956" t="inlineStr">
+        <is>
+          <t>K9606VIP3</t>
+        </is>
+      </c>
+      <c r="B1956" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1956">
+        <v>4.69</v>
+      </c>
+      <c r="D1956">
+        <v>6</v>
+      </c>
+      <c r="E1956" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1957">
+      <c r="A1957" t="inlineStr">
+        <is>
+          <t>MG580PWU</t>
+        </is>
+      </c>
+      <c r="B1957" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1957">
+        <v>4.69</v>
+      </c>
+      <c r="D1957">
+        <v>6</v>
+      </c>
+      <c r="E1957" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1958">
+      <c r="A1958" t="inlineStr">
+        <is>
+          <t>MG593PWU</t>
+        </is>
+      </c>
+      <c r="B1958" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1958">
+        <v>3.99</v>
+      </c>
+      <c r="D1958">
+        <v>6</v>
+      </c>
+      <c r="E1958" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1959">
+      <c r="A1959" t="inlineStr">
+        <is>
+          <t>MG652PWU</t>
+        </is>
+      </c>
+      <c r="B1959" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1959">
+        <v>4.16</v>
+      </c>
+      <c r="D1959">
+        <v>6</v>
+      </c>
+      <c r="E1959" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1960">
+      <c r="A1960" t="inlineStr">
+        <is>
+          <t>NK506VIP3</t>
+        </is>
+      </c>
+      <c r="B1960" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1960">
+        <v>4.34</v>
+      </c>
+      <c r="D1960">
+        <v>6</v>
+      </c>
+      <c r="E1960" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1961">
+      <c r="A1961" t="inlineStr">
+        <is>
+          <t>NK508</t>
+        </is>
+      </c>
+      <c r="B1961" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1961">
+        <v>3.81</v>
+      </c>
+      <c r="D1961">
+        <v>6</v>
+      </c>
+      <c r="E1961" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1962">
+      <c r="A1962" t="inlineStr">
+        <is>
+          <t>NK511VIP3</t>
+        </is>
+      </c>
+      <c r="B1962" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1962">
+        <v>5.38</v>
+      </c>
+      <c r="D1962">
+        <v>6</v>
+      </c>
+      <c r="E1962" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1963">
+      <c r="A1963" t="inlineStr">
+        <is>
+          <t>NK520VIP3</t>
+        </is>
+      </c>
+      <c r="B1963" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1963">
+        <v>4.69</v>
+      </c>
+      <c r="D1963">
+        <v>6</v>
+      </c>
+      <c r="E1963" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1964">
+      <c r="A1964" t="inlineStr">
+        <is>
+          <t>NK555VIP3</t>
+        </is>
+      </c>
+      <c r="B1964" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1964">
+        <v>5.64</v>
+      </c>
+      <c r="D1964">
+        <v>6</v>
+      </c>
+      <c r="E1964" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1965">
+      <c r="A1965" t="inlineStr">
+        <is>
+          <t>NS75VIP3</t>
+        </is>
+      </c>
+      <c r="B1965" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1965">
+        <v>4.86</v>
+      </c>
+      <c r="D1965">
+        <v>6</v>
+      </c>
+      <c r="E1965" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1966">
+      <c r="A1966" t="inlineStr">
+        <is>
+          <t>NS80VIP3</t>
+        </is>
+      </c>
+      <c r="B1966" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1966">
+        <v>5.38</v>
+      </c>
+      <c r="D1966">
+        <v>6</v>
+      </c>
+      <c r="E1966" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1967">
+      <c r="A1967" t="inlineStr">
+        <is>
+          <t>NS88VIP3</t>
+        </is>
+      </c>
+      <c r="B1967" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1967">
+        <v>4.51</v>
+      </c>
+      <c r="D1967">
+        <v>6</v>
+      </c>
+      <c r="E1967" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1968">
+      <c r="A1968" t="inlineStr">
+        <is>
+          <t>NS90PRO2</t>
+        </is>
+      </c>
+      <c r="B1968" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1968">
+        <v>3.99</v>
+      </c>
+      <c r="D1968">
+        <v>6</v>
+      </c>
+      <c r="E1968" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1969">
+      <c r="A1969" t="inlineStr">
+        <is>
+          <t>NS91VIP2</t>
+        </is>
+      </c>
+      <c r="B1969" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1969">
+        <v>4.86</v>
+      </c>
+      <c r="D1969">
+        <v>6</v>
+      </c>
+      <c r="E1969" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1970">
+      <c r="A1970" t="inlineStr">
+        <is>
+          <t>NS91VIP3</t>
+        </is>
+      </c>
+      <c r="B1970" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1970">
+        <v>4.69</v>
+      </c>
+      <c r="D1970">
+        <v>6</v>
+      </c>
+      <c r="E1970" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1971">
+      <c r="A1971" t="inlineStr">
+        <is>
+          <t>NS95VIP2</t>
+        </is>
+      </c>
+      <c r="B1971" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1971">
+        <v>5.21</v>
+      </c>
+      <c r="D1971">
+        <v>6</v>
+      </c>
+      <c r="E1971" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1972">
+      <c r="A1972" t="inlineStr">
+        <is>
+          <t>P3707VYH</t>
+        </is>
+      </c>
+      <c r="B1972" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1972">
+        <v>4.86</v>
+      </c>
+      <c r="D1972">
+        <v>6</v>
+      </c>
+      <c r="E1972" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1973">
+      <c r="A1973" t="inlineStr">
+        <is>
+          <t>P3845VYHR</t>
+        </is>
+      </c>
+      <c r="B1973" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1973">
+        <v>5.38</v>
+      </c>
+      <c r="D1973">
+        <v>6</v>
+      </c>
+      <c r="E1973" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1974">
+      <c r="A1974" t="inlineStr">
+        <is>
+          <t>P3858PWU</t>
+        </is>
+      </c>
+      <c r="B1974" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1974">
+        <v>5.21</v>
+      </c>
+      <c r="D1974">
+        <v>6</v>
+      </c>
+      <c r="E1974" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1975">
+      <c r="A1975" t="inlineStr">
+        <is>
+          <t>P3889RR</t>
+        </is>
+      </c>
+      <c r="B1975" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1975">
+        <v>4.86</v>
+      </c>
+      <c r="D1975">
+        <v>6</v>
+      </c>
+      <c r="E1975" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1976">
+      <c r="A1976" t="inlineStr">
+        <is>
+          <t>P3898</t>
+        </is>
+      </c>
+      <c r="B1976" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1976">
+        <v>5.21</v>
+      </c>
+      <c r="D1976">
+        <v>6</v>
+      </c>
+      <c r="E1976" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1977">
+      <c r="A1977" t="inlineStr">
+        <is>
+          <t>STATUSVIP3</t>
+        </is>
+      </c>
+      <c r="B1977" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1977">
+        <v>3.99</v>
+      </c>
+      <c r="D1977">
+        <v>6</v>
+      </c>
+      <c r="E1977" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1978">
+      <c r="A1978" t="inlineStr">
+        <is>
+          <t>SXC2251TG.0</t>
+        </is>
+      </c>
+      <c r="B1978" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1978">
+        <v>4.51</v>
+      </c>
+      <c r="D1978">
+        <v>6</v>
+      </c>
+      <c r="E1978" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1979">
+      <c r="A1979" t="inlineStr">
+        <is>
+          <t>SXC2251ZL.0</t>
+        </is>
+      </c>
+      <c r="B1979" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1979">
+        <v>4.34</v>
+      </c>
+      <c r="D1979">
+        <v>6</v>
+      </c>
+      <c r="E1979" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1980">
+      <c r="A1980" t="inlineStr">
+        <is>
+          <t>SXC2320VIP3</t>
+        </is>
+      </c>
+      <c r="B1980" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1980">
+        <v>4.86</v>
+      </c>
+      <c r="D1980">
+        <v>6</v>
+      </c>
+      <c r="E1980" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1981">
+      <c r="A1981" t="inlineStr">
+        <is>
+          <t>SXD2621ZL.0</t>
+        </is>
+      </c>
+      <c r="B1981" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1981">
+        <v>3.99</v>
+      </c>
+      <c r="D1981">
+        <v>6</v>
+      </c>
+      <c r="E1981" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1982">
+      <c r="A1982" t="inlineStr">
+        <is>
+          <t>SYC7131ZL.0</t>
+        </is>
+      </c>
+      <c r="B1982" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1982">
+        <v>3.99</v>
+      </c>
+      <c r="D1982">
+        <v>6</v>
+      </c>
+      <c r="E1982" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1983">
+      <c r="A1983" t="inlineStr">
+        <is>
+          <t>SYC7441ZL.0</t>
+        </is>
+      </c>
+      <c r="B1983" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1983">
+        <v>5.04</v>
+      </c>
+      <c r="D1983">
+        <v>6</v>
+      </c>
+      <c r="E1983" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1984">
+      <c r="A1984" t="inlineStr">
+        <is>
+          <t>SZC4141ZL.0</t>
+        </is>
+      </c>
+      <c r="B1984" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1984">
+        <v>4.86</v>
+      </c>
+      <c r="D1984">
+        <v>6</v>
+      </c>
+      <c r="E1984" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1985">
+      <c r="A1985" t="inlineStr">
+        <is>
+          <t>SZD5031ZL.0</t>
+        </is>
+      </c>
+      <c r="B1985" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1985">
+        <v>3.99</v>
+      </c>
+      <c r="D1985">
+        <v>6</v>
+      </c>
+      <c r="E1985" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1986">
+      <c r="A1986" t="inlineStr">
+        <is>
+          <t>SZD5211ZL.0</t>
+        </is>
+      </c>
+      <c r="B1986" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1986">
+        <v>4.86</v>
+      </c>
+      <c r="D1986">
+        <v>6</v>
+      </c>
+      <c r="E1986" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1987">
+      <c r="A1987" t="inlineStr">
+        <is>
+          <t>SZE6111TG.0</t>
+        </is>
+      </c>
+      <c r="B1987" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1987">
+        <v>3.99</v>
+      </c>
+      <c r="D1987">
+        <v>6</v>
+      </c>
+      <c r="E1987" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1988">
+      <c r="A1988" t="inlineStr">
+        <is>
+          <t>SZE6111VIP3</t>
+        </is>
+      </c>
+      <c r="B1988" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1988">
+        <v>3.99</v>
+      </c>
+      <c r="D1988">
+        <v>6</v>
+      </c>
+      <c r="E1988" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1989">
+      <c r="A1989" t="inlineStr">
+        <is>
+          <t>SZF6101VIP3</t>
+        </is>
+      </c>
+      <c r="B1989" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1989">
+        <v>3.64</v>
+      </c>
+      <c r="D1989">
+        <v>6</v>
+      </c>
+      <c r="E1989" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1990">
+      <c r="A1990" t="inlineStr">
+        <is>
+          <t>SZF6101WT.0</t>
+        </is>
+      </c>
+      <c r="B1990" t="inlineStr">
+        <is>
+          <t>22WNBPEYG6K1BU35</t>
+        </is>
+      </c>
+      <c r="C1990">
+        <v>3.64</v>
+      </c>
+      <c r="D1990">
+        <v>6</v>
+      </c>
+      <c r="E1990" t="inlineStr">
+        <is>
+          <t>trial</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>